<commit_message>
fixed reports endpoints, updated documentation, added login endpont for /users, added check to see if email is already registered, added method to search all reports by an specifc userd
</commit_message>
<xml_diff>
--- a/Endpoints GS2.xlsx
+++ b/Endpoints GS2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\supev\Documents\EOQ\FIAP\1TDSPM\Global Solution 2\Java\gslevi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB333738-C20E-4162-8C75-FB83D39B6AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E913E8BE-137A-49D4-9021-2802C9520E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>/regions</t>
   </si>
@@ -169,6 +169,27 @@
   </si>
   <si>
     <t>HTTP</t>
+  </si>
+  <si>
+    <t>/users/login</t>
+  </si>
+  <si>
+    <t>Recebe um JSON como body, retorna as infos do usuário tenha sucesso, ou acesso negado caso contrário.</t>
+  </si>
+  <si>
+    <t>/reports?user={id}</t>
+  </si>
+  <si>
+    <t>Retorna todos os relatórios de um usuário com id = {id} em JSON</t>
+  </si>
+  <si>
+    <t>500 - "Erro ao tentar logar..."</t>
+  </si>
+  <si>
+    <t>401 - Email ou senha inválidos..."</t>
+  </si>
+  <si>
+    <t>200 - Usuário é logado</t>
   </si>
 </sst>
 </file>
@@ -261,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -491,11 +512,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -541,7 +588,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -559,6 +605,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D11:I27"/>
+  <dimension ref="D11:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,169 +1033,212 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="14" t="s">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D18" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I19" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="17"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="20"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D20" s="21" t="s">
+    <row r="20" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E21" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F21" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G21" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H21" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="25" t="s">
+      <c r="I21" s="25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="15" t="s">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E22" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H23" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I23" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="27"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="28" t="s">
+    <row r="24" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E25" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F25" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G25" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="24" t="s">
+      <c r="H25" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I25" s="25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="31" t="s">
+    <row r="26" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E26" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F26" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G26" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I26" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D26" s="34" t="s">
+    <row r="27" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D28" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E28" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F28" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="23" t="s">
+      <c r="G28" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="H28" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="25" t="s">
+      <c r="I28" s="25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="9" t="s">
+    <row r="29" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F29" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G29" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H29" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="I29" s="12" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H32" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed passing IdRegiao as IdUsuario and vice versa on RelatorioDAO
</commit_message>
<xml_diff>
--- a/Endpoints GS2.xlsx
+++ b/Endpoints GS2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\supev\Documents\EOQ\FIAP\1TDSPM\Global Solution 2\Java\gslevi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E913E8BE-137A-49D4-9021-2802C9520E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5877D494-C1A2-4DC6-9D64-0398759CCA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,7 +905,7 @@
   <dimension ref="D11:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated dependencies, endpoints sheet, redeployed
</commit_message>
<xml_diff>
--- a/Endpoints GS2.xlsx
+++ b/Endpoints GS2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\supev\Documents\EOQ\FIAP\1TDSPM\Global Solution 2\Java\gslevi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5877D494-C1A2-4DC6-9D64-0398759CCA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149B0AE6-5564-49F4-A0CA-3AD12FF2CC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,7 +905,7 @@
   <dimension ref="D11:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>